<commit_message>
Added tests for worksheet cell protection.
</commit_message>
<xml_diff>
--- a/test/perl_output/protection.xlsx
+++ b/test/perl_output/protection.xlsx
@@ -64,10 +64,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection hidden="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -396,7 +399,7 @@
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="2">
         <f>1+2</f>
         <v>3</v>
       </c>

</xml_diff>